<commit_message>
Finished lab4, added lab7, started project
</commit_message>
<xml_diff>
--- a/Lab4/ex2.xlsx
+++ b/Lab4/ex2.xlsx
@@ -379,7 +379,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,6 +388,9 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>